<commit_message>
11-practice: food order app
</commit_message>
<xml_diff>
--- a/ReactJS.xlsx
+++ b/ReactJS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\202301_ReactJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F73664-DC72-4D1A-8760-70B95B7EB038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FF4394-DFA5-4649-924C-E3ABCE8E5F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="525" windowWidth="15375" windowHeight="7875" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -22,11 +22,12 @@
     <sheet name="10.useEffect" sheetId="6" r:id="rId7"/>
     <sheet name="10.useReducer" sheetId="12" r:id="rId8"/>
     <sheet name="10.useContext" sheetId="13" r:id="rId9"/>
-    <sheet name="13.ClassLifecycle" sheetId="8" r:id="rId10"/>
-    <sheet name="14.http" sheetId="14" r:id="rId11"/>
-    <sheet name="21.Deploy" sheetId="10" r:id="rId12"/>
-    <sheet name="DOM" sheetId="5" r:id="rId13"/>
-    <sheet name="Hooks" sheetId="7" r:id="rId14"/>
+    <sheet name="12.Optimization" sheetId="15" r:id="rId10"/>
+    <sheet name="13.ClassLifecycle" sheetId="8" r:id="rId11"/>
+    <sheet name="14.http" sheetId="14" r:id="rId12"/>
+    <sheet name="21.Deploy" sheetId="10" r:id="rId13"/>
+    <sheet name="DOM" sheetId="5" r:id="rId14"/>
+    <sheet name="Hooks" sheetId="7" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="1041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="1099">
   <si>
     <t>React - The Complete Guide (incl Hooks, React Router, Redux)</t>
   </si>
@@ -3192,21 +3193,12 @@
     <t>Deployment Steps</t>
   </si>
   <si>
-    <t>Test Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optimize Code </t>
-  </si>
-  <si>
     <t>Build App for Production</t>
   </si>
   <si>
     <t>Upload Production Code to Server</t>
   </si>
   <si>
-    <t>Configure Server</t>
-  </si>
-  <si>
     <t>(Lazy loading)</t>
   </si>
   <si>
@@ -3253,9 +3245,6 @@
   </si>
   <si>
     <t>build: react-scripts build</t>
-  </si>
-  <si>
-    <t>-&gt; $ npm run build</t>
   </si>
   <si>
     <t>-&gt; build folder</t>
@@ -4870,13 +4859,450 @@
   </si>
   <si>
     <t xml:space="preserve">    console.log(data);</t>
+  </si>
+  <si>
+    <t>1. Test Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Optimize Code </t>
+  </si>
+  <si>
+    <t>3. Build App for Production</t>
+  </si>
+  <si>
+    <t>4. Upload Production Code to Server</t>
+  </si>
+  <si>
+    <t>5. Configure Server</t>
+  </si>
+  <si>
+    <t>npm run build</t>
+  </si>
+  <si>
+    <t>-&gt; npm run build</t>
+  </si>
+  <si>
+    <t>How does React work behind the scene?</t>
+  </si>
+  <si>
+    <t>Understand the Virtual DOM &amp; DOM updates</t>
+  </si>
+  <si>
+    <t>Understand State &amp; State updates</t>
+  </si>
+  <si>
+    <t>12.Optimization</t>
+  </si>
+  <si>
+    <t>How does React work?</t>
+  </si>
+  <si>
+    <t>React xác định component tree hiện tại như thế nào và sẽ trông như thế nào</t>
+  </si>
+  <si>
+    <t>ReactDOM nhận sự thay đổi và điều khiển RealDOM</t>
+  </si>
+  <si>
+    <t>Re-Evaluating Components !== Re-rendering the DOM</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>Real DOM</t>
+  </si>
+  <si>
+    <t>Chỉ thay đổi khi có sự khác biệt sau khi evaluate</t>
+  </si>
+  <si>
+    <t>Re-evaluated mỗi khi props, state hoặc context thay đổi</t>
+  </si>
+  <si>
+    <t>React execute các component functions!</t>
+  </si>
+  <si>
+    <t>=&gt; prevent unnecessary re-evaluation</t>
+  </si>
+  <si>
+    <t>React.memo()</t>
+  </si>
+  <si>
+    <t>Ngăn ngừa việc re-evaluation không cần thiết.</t>
+  </si>
+  <si>
+    <t>=&gt; dù props.show là cố định, nhưng Demo component vẫn bị re-render mỗi khi App re-render</t>
+  </si>
+  <si>
+    <t>Áp dụng:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">export default </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>React.memo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Demo);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;Demo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>show={true}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> /&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Chỉ có kiểu primitive (boolean, string,…) mới là không đổi </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">T/h2 : Khi props là một function -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function luôn được tạo mới</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> mỗi khi parent component re-render</t>
+    </r>
+  </si>
+  <si>
+    <t>=&gt; Button component luôn được re-render khi parent component re-render</t>
+  </si>
+  <si>
+    <t>React.memo, useCallback, useMemo</t>
+  </si>
+  <si>
+    <t>Ví dụ: Khi App component truyền props vào Demo component</t>
+  </si>
+  <si>
+    <t>useCallback()</t>
+  </si>
+  <si>
+    <t>Là một React hook</t>
+  </si>
+  <si>
+    <t>trả về cùng một function giống nhau khi được gọi.</t>
+  </si>
+  <si>
+    <t>=&gt; Cần áp dụng pp khác: useCallback()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Behind the scene: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    setShowPara(prevState =&gt; !prevState);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  }, []);</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Button onClick={</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>toggleParagraphHandler</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}&gt;Toggle Paragraph&lt;/Button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  const </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>toggleParagraphHandler</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>useCallback</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(() =&gt; {</t>
+    </r>
+  </si>
+  <si>
+    <t>=&gt; Hạn chế việc re-render không cần thiết</t>
+  </si>
+  <si>
+    <t>useCallback() và Dependencies</t>
+  </si>
+  <si>
+    <t>Khi sử dụng useCallback, các function bao gồm cả các biến bên trong nó được giữ nguyên.</t>
+  </si>
+  <si>
+    <t>=&gt; VẤN ĐỀ: biến không được update khi state thay đổi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      setShowPara(prevState =&gt; !prevState);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    if (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>allowToggle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  const [allowToggle, setAllowToggle] = useState(false);</t>
+  </si>
+  <si>
+    <t>//biến này không đổi khi state update</t>
+  </si>
+  <si>
+    <t>=&gt; Sử dụng Dependency: tạo lại function khi dependency thay đổi.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  }, [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>allowToggle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]);</t>
+    </r>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/JavaScript/Closures</t>
+  </si>
+  <si>
+    <t>//tạo function mới khi state update</t>
+  </si>
+  <si>
+    <t>useMemo()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">chứa </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> vào trong React internal</t>
+    </r>
+  </si>
+  <si>
+    <t>memorize/store data: array, object, expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  return items.sort((a, b) =&gt; a - b);</t>
+  </si>
+  <si>
+    <t>}, [items]);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">const sortedList = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>useMemo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(() =&gt; {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">const listItems = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>useMemo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(() =&gt; { return [1, 2, 3]; }, []);</t>
+    </r>
+  </si>
+  <si>
+    <t>Section 17</t>
+  </si>
+  <si>
+    <t>Practice 3: Adding http &amp; forms to food order app</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5054,6 +5480,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5082,7 +5516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -5123,6 +5557,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5481,6 +5916,749 @@
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>291352</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="923458" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80008845-0745-4F28-A750-FD8BF89A8063}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8762999" y="3249706"/>
+          <a:ext cx="923458" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Internal data</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>251011</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>183777</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Rectangle 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB3B22B7-054C-4961-8355-8F096CC1594F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7512423" y="2290483"/>
+          <a:ext cx="1187824" cy="549088"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Components</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>235323</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>251012</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Rectangle 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{127DF756-27B5-46F6-93CE-C976AECECCD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7496735" y="1535206"/>
+          <a:ext cx="1225924" cy="351865"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Context</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>239806</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>172571</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>255495</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>143436</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Rectangle 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63A31F63-2505-44BA-8D4E-35785DC56EC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7501218" y="3231777"/>
+          <a:ext cx="1225924" cy="351865"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>State</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>239806</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>127748</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>255495</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>98613</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Rectangle 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09C7E1D0-D6DC-428C-A06E-B58D520C1407}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5685865" y="2424954"/>
+          <a:ext cx="1225924" cy="351865"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Props</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>235323</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>183778</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>575981</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>172572</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Rectangle 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EC330A5-09FF-4575-8FFB-839C32DA8011}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9312088" y="2290484"/>
+          <a:ext cx="1550893" cy="560294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Real DOM</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>what</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> the user sees</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>239806</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>60512</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Arrow: Right 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F80EF576-EF20-458A-AE72-9F465805C9F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6694395" y="2458571"/>
+          <a:ext cx="806823" cy="280147"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>52668</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>86288</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>417980</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>49310</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Arrow: Right 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C210D1BD-17B6-4E49-9F72-6AA103E3C716}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7834592" y="1896599"/>
+          <a:ext cx="534522" cy="365312"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>48185</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104218</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>413497</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>67240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="Arrow: Right 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46C71D10-747A-4A57-819C-ABFFAACCCBF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="7830109" y="2867029"/>
+          <a:ext cx="534522" cy="365312"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>206189</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1470339" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="TextBox 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{517FEE50-B17C-4BE6-A94F-6546157B7BA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8677836" y="1573306"/>
+          <a:ext cx="1470339" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Component-wide</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> data</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>156883</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1872116" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="TextBox 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A74415FC-58C2-4E1D-A26B-7197EC9E1DA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5446059" y="2835089"/>
+          <a:ext cx="1872116" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> from parent component</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>172571</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>138952</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>257736</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="Arrow: Right 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0ACD1CC9-E5FA-46D4-A5D2-40ABD4430482}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8644218" y="2436158"/>
+          <a:ext cx="690283" cy="275665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 58000"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
@@ -5545,7 +6723,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -5594,7 +6772,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -5994,10 +7172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:R39"/>
+  <dimension ref="B2:R40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6034,7 +7212,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="K8" s="29">
         <v>44906</v>
@@ -6048,7 +7226,7 @@
         <v>6</v>
       </c>
       <c r="J9" s="30" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="K9" s="29">
         <v>44914</v>
@@ -6062,7 +7240,7 @@
         <v>7</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="K10" s="29">
         <v>44928</v>
@@ -6076,7 +7254,7 @@
         <v>22</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="K11" s="29">
         <v>44938</v>
@@ -6095,10 +7273,10 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C13" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="K13" s="29">
         <v>44940</v>
@@ -6109,10 +7287,10 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="K14" s="29">
         <v>44940</v>
@@ -6123,10 +7301,10 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="K15" s="29">
         <v>44940</v>
@@ -6134,10 +7312,10 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="J16" s="30" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="K16" s="29">
         <v>44941</v>
@@ -6145,10 +7323,10 @@
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="J17" s="30" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="K17" s="29">
         <v>44941</v>
@@ -6156,10 +7334,10 @@
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="C18" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="J18" s="30"/>
     </row>
@@ -6170,6 +7348,12 @@
       <c r="C19" t="s">
         <v>24</v>
       </c>
+      <c r="J19" s="30" t="s">
+        <v>1047</v>
+      </c>
+      <c r="K19" s="29">
+        <v>44943</v>
+      </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -6179,7 +7363,7 @@
         <v>25</v>
       </c>
       <c r="J20" s="30" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="K20" s="29">
         <v>44942</v>
@@ -6193,7 +7377,10 @@
         <v>26</v>
       </c>
       <c r="J21" s="30" t="s">
-        <v>990</v>
+        <v>986</v>
+      </c>
+      <c r="K21" s="29">
+        <v>44942</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
@@ -6214,152 +7401,160 @@
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>19</v>
+        <v>1097</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>55</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
-      </c>
-      <c r="M25" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M26" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
-      </c>
-      <c r="J27" s="30" t="s">
-        <v>703</v>
-      </c>
-      <c r="K27" s="29">
-        <v>44930</v>
+        <v>31</v>
       </c>
       <c r="M27" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="J28" s="30" t="s">
+        <v>703</v>
+      </c>
+      <c r="K28" s="29">
+        <v>44930</v>
       </c>
       <c r="M28" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="M29" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="R30" t="s">
-        <v>468</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>332</v>
+        <v>285</v>
       </c>
       <c r="R31" t="s">
-        <v>409</v>
+        <v>468</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
-      </c>
-      <c r="M32" t="s">
-        <v>661</v>
+        <v>44</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="R32" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M33" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="M34" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>47</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>470</v>
       </c>
-      <c r="K38" s="22">
+      <c r="K39" s="22">
         <v>44924</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="K39" s="22">
+      <c r="K40" s="22">
         <v>44564</v>
       </c>
     </row>
@@ -6367,21 +7562,22 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{CAC955B5-BA63-49AE-8455-DCB0484BB07B}"/>
-    <hyperlink ref="M24" r:id="rId2" xr:uid="{67E7922B-6A2B-4AEB-9D38-04EF21365958}"/>
-    <hyperlink ref="M30" r:id="rId3" xr:uid="{AA4F42E1-CA21-4C81-AF61-E929D299C8BC}"/>
-    <hyperlink ref="M31" r:id="rId4" location="installation" xr:uid="{4C33BC18-1571-47C0-BCC4-2DB536B9BC45}"/>
-    <hyperlink ref="B39" r:id="rId5" xr:uid="{53C62C83-76F9-4302-8049-1D9F2F43DDF9}"/>
+    <hyperlink ref="M25" r:id="rId2" xr:uid="{67E7922B-6A2B-4AEB-9D38-04EF21365958}"/>
+    <hyperlink ref="M31" r:id="rId3" xr:uid="{AA4F42E1-CA21-4C81-AF61-E929D299C8BC}"/>
+    <hyperlink ref="M32" r:id="rId4" location="installation" xr:uid="{4C33BC18-1571-47C0-BCC4-2DB536B9BC45}"/>
+    <hyperlink ref="B40" r:id="rId5" xr:uid="{53C62C83-76F9-4302-8049-1D9F2F43DDF9}"/>
     <hyperlink ref="J8" location="'3.Component'!A1" display="3.Component" xr:uid="{9F9F9AE5-459C-4DA1-BCBE-AFC3896C5272}"/>
     <hyperlink ref="J9" location="'4.useState'!A1" display="4.useState" xr:uid="{A379BE02-A27A-4D88-9249-8432494B7DDC}"/>
     <hyperlink ref="J10" location="'5.RenderList'!A1" display="5.RenderList" xr:uid="{C4A1AE85-944E-463F-A842-68F12863221E}"/>
     <hyperlink ref="J11" location="'6.Style'!A1" display="6.Style" xr:uid="{07D61642-9F57-491A-94DE-B2E82B426AE2}"/>
     <hyperlink ref="J15" location="'10.UseEffect'!A1" display="10.UseEffect" xr:uid="{89550841-E73A-4F06-9FD2-81617C48C729}"/>
-    <hyperlink ref="J27" location="'21.Deploy'!A1" display="21.Deploy" xr:uid="{A1608A3A-4F55-4EEF-96B9-E79B3A050F13}"/>
+    <hyperlink ref="J28" location="'21.Deploy'!A1" display="21.Deploy" xr:uid="{A1608A3A-4F55-4EEF-96B9-E79B3A050F13}"/>
     <hyperlink ref="J14" location="'9.Fragment'!A1" display="'9.Fragment" xr:uid="{B4CB4FC9-B32F-4AA9-BF3F-141874CB2631}"/>
     <hyperlink ref="J16" location="'10.useReducer'!A1" display="'10.useReducer" xr:uid="{5685383D-A2FA-4EC3-82D9-7362046D59C5}"/>
     <hyperlink ref="J17" location="'10.useContext'!A1" display="'10.useContext" xr:uid="{205D2731-DB42-4462-9AF5-859F910E58D6}"/>
     <hyperlink ref="J20" location="'13.ClassLifecycle'!A1" display="'13.ClassLifecycle" xr:uid="{896D7DA3-33BE-47E7-8E25-D72BCC04B8F8}"/>
     <hyperlink ref="J21" location="'14.http'!A1" display="'14.http" xr:uid="{0A522652-D386-4F99-998C-E844A21B255E}"/>
+    <hyperlink ref="J19" location="'12.Optimization'!A1" display="'12.Optimization" xr:uid="{427A2453-5E42-49EE-AF1C-B9FE524201AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
@@ -6390,6 +7586,319 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CA327F-B97A-4665-A7A7-EF09848B5E27}">
+  <dimension ref="A1:I66"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1045</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="4" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="16" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="16" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="9" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="6" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="9" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E32" s="9" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="6" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="6" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="13" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="6" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C49" s="6" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C50" s="6"/>
+      <c r="D50" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>1083</v>
+      </c>
+      <c r="I52" s="38" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C56" s="6" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>1087</v>
+      </c>
+      <c r="I57" s="38" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="13" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Intro!A1" display="Intro" xr:uid="{68F65D08-56FD-4495-900A-E979F99C094A}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{BD1AB6BB-3E25-4768-ACCF-0116F248D86E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{818115DD-5FA9-495E-93E6-8A4516AFECDE}">
   <dimension ref="A1:M94"/>
   <sheetViews>
@@ -6417,22 +7926,22 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -6440,7 +7949,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -6548,10 +8057,10 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D36" s="25" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="J36" s="31" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
@@ -6648,7 +8157,7 @@
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D51" s="6" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="M51" t="s">
         <v>592</v>
@@ -6816,7 +8325,7 @@
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C71" s="14" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
       <c r="M71" t="s">
         <v>606</v>
@@ -6837,7 +8346,7 @@
     </row>
     <row r="75" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="C75" s="19"/>
       <c r="D75" s="19"/>
@@ -6853,7 +8362,7 @@
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
       <c r="M76" t="s">
         <v>609</v>
@@ -6861,7 +8370,7 @@
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
       <c r="M77" t="s">
         <v>125</v>
@@ -6874,18 +8383,18 @@
     </row>
     <row r="79" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C79" s="16" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="H79" s="16" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="H80" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="M80" t="s">
         <v>610</v>
@@ -6896,7 +8405,7 @@
         <v>595</v>
       </c>
       <c r="H81" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
       <c r="M81" t="s">
         <v>611</v>
@@ -6904,7 +8413,7 @@
     </row>
     <row r="82" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="H82" t="s">
         <v>75</v>
@@ -6925,42 +8434,42 @@
     </row>
     <row r="86" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
     </row>
     <row r="87" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D87" s="36" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
     </row>
     <row r="88" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D88" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
     </row>
     <row r="89" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D89" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
     </row>
     <row r="91" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B91" s="4" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
     </row>
     <row r="92" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
     </row>
     <row r="93" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D93" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
     </row>
     <row r="94" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
     </row>
   </sheetData>
@@ -6975,13 +8484,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8615145-4EC8-409D-9AD0-4BE86352B7C9}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -6992,20 +8499,20 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -7018,221 +8525,221 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="I25" s="31" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
@@ -7242,12 +8749,12 @@
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.25">
@@ -7267,11 +8774,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F33E95-6BA3-4923-8488-FAE427356E73}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -7283,7 +8792,7 @@
         <v>704</v>
       </c>
       <c r="H1" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -7314,85 +8823,88 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>708</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>709</v>
-      </c>
-      <c r="E11" t="s">
-        <v>713</v>
+        <v>1038</v>
+      </c>
+      <c r="G11" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>710</v>
+        <v>1039</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1042</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>711</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>712</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D24" s="9" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -7402,122 +8914,122 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C36" s="32" t="s">
-        <v>729</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C37" s="6" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C42" s="25" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C48" s="10" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="6" t="s">
+        <v>735</v>
+      </c>
+      <c r="G49" s="6" t="s">
         <v>739</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="6" t="s">
+        <v>736</v>
+      </c>
+      <c r="G50" s="6" t="s">
         <v>740</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="G51" s="6" t="s">
         <v>741</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="6" t="s">
+        <v>738</v>
+      </c>
+      <c r="G52" s="6" t="s">
         <v>742</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G53" s="6" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G54" s="6" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
   </sheetData>
@@ -7529,7 +9041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A1AAE5-8895-4972-BA44-ABCE854AC42B}">
   <dimension ref="B2:S271"/>
   <sheetViews>
@@ -8629,12 +10141,12 @@
     </row>
     <row r="220" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D220" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
     </row>
     <row r="221" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D221" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
     </row>
     <row r="222" spans="3:10" x14ac:dyDescent="0.25">
@@ -8928,7 +10440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D9D265-7661-41E2-8F58-51E51B362C39}">
   <dimension ref="B1:G39"/>
   <sheetViews>
@@ -8950,7 +10462,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
     </row>
     <row r="8" spans="2:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -8984,7 +10496,7 @@
         <v>516</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
@@ -8992,7 +10504,7 @@
         <v>517</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -9005,7 +10517,7 @@
         <v>519</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -9023,7 +10535,7 @@
         <v>522</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -9031,7 +10543,7 @@
         <v>523</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -9071,42 +10583,42 @@
     </row>
     <row r="32" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="13" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
     </row>
   </sheetData>
@@ -9120,7 +10632,7 @@
   <dimension ref="B1:H72"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9145,17 +10657,17 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -10344,7 +11856,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -10562,152 +12074,152 @@
     <row r="8" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
   </sheetData>
@@ -10737,17 +12249,17 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -10755,68 +12267,68 @@
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" s="6" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D20" s="9" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="H20" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D21" s="9" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -10824,138 +12336,138 @@
         <v>75</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D23" s="9" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="H23" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D28" s="8" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D29" s="9" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D30" s="9" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D31" s="8" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
     </row>
     <row r="34" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="13" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
     </row>
     <row r="40" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D40" s="21" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D42" s="24" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="M42" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D43" s="24" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D46" s="4" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
@@ -10965,32 +12477,32 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
@@ -11000,62 +12512,62 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="62" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="13" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C63" s="5" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
     </row>
   </sheetData>
@@ -11095,7 +12607,7 @@
         <v>376</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -11118,7 +12630,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -11158,17 +12670,17 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D19" s="6" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D20" s="6" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -11432,42 +12944,42 @@
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
     </row>
   </sheetData>
@@ -11497,18 +13009,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -11518,92 +13030,92 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D12" s="21" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="F14" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="F15" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
       <c r="F16" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
       <c r="F20" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="K24" s="31" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
@@ -11613,15 +13125,15 @@
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="K29" s="31" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
@@ -11631,37 +13143,37 @@
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
@@ -11671,30 +13183,30 @@
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="K40" s="31" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
@@ -11704,39 +13216,39 @@
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C47" s="16" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="H48" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="H49" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="H50" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -11752,7 +13264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3BEAA15-8479-45BC-B250-088745942515}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -11765,18 +13277,18 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C10" s="37" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -11786,53 +13298,53 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
@@ -11842,37 +13354,37 @@
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D29" s="4" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
@@ -11882,57 +13394,57 @@
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="13" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>